<commit_message>
Add data check script
</commit_message>
<xml_diff>
--- a/results/Corrs_table.xlsx
+++ b/results/Corrs_table.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -53,74 +53,6 @@
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -424,7 +356,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>cdwa_v0_a0_b0</t>
+          <t>cdwa1</t>
         </is>
       </c>
     </row>
@@ -473,23 +405,23 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>0.4689104025791357</v>
+        <v>0.5735415670576476</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2553553282037202</v>
+        <v>0.3892947992043204</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3742863803593708</v>
+        <v>0.4141080527342521</v>
       </c>
       <c r="E4" t="n">
-        <v>0.357250055714746</v>
+        <v>0.3219275759755983</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5687094947327561</v>
+        <v>0.6936566612013039</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>exp2_cdwa_v0_a0_b0_w3_C4_r0.bag</t>
+          <t>exp3_cdwa1_w3_C4_r0.bag</t>
         </is>
       </c>
     </row>
@@ -498,23 +430,23 @@
         <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.3215713768388223</v>
+        <v>-0.4250783238122718</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.1991424805223243</v>
+        <v>-0.5524747170534537</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.09745590652710043</v>
+        <v>-0.5392094904281148</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1746255222418195</v>
+        <v>0.2737667704825002</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.3294460849901111</v>
+        <v>-0.3407558095979445</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>exp2_cdwa_v0_a0_b0_w3_C4_r1.bag</t>
+          <t>exp3_cdwa1_w3_C4_r1.bag</t>
         </is>
       </c>
     </row>
@@ -523,23 +455,23 @@
         <v>2</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.3305726354464067</v>
+        <v>-0.3247574537317936</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.4566258477853971</v>
+        <v>-0.472956243854587</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.5207720410089315</v>
+        <v>-0.5597554112639272</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.4578146885444032</v>
+        <v>-0.5063208533582128</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.3174738078995539</v>
+        <v>-0.328693297293293</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>exp2_cdwa_v0_a0_b0_w3_C4_r2.bag</t>
+          <t>exp3_cdwa1_w3_C4_r2.bag</t>
         </is>
       </c>
     </row>
@@ -548,23 +480,23 @@
         <v>3</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1686980594547547</v>
+        <v>-0.1926057445151897</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2467729028088164</v>
+        <v>-0.3852435535824921</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3968186880128692</v>
+        <v>-0.4674057805024837</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3570433571055948</v>
+        <v>-0.3893843817353697</v>
       </c>
       <c r="F7" t="n">
-        <v>0.222028201101028</v>
+        <v>-0.2672051563932004</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>exp2_cdwa_v0_a0_b0_w3_C4_r3.bag</t>
+          <t>exp3_cdwa1_w3_C4_r3.bag</t>
         </is>
       </c>
     </row>
@@ -573,23 +505,23 @@
         <v>4</v>
       </c>
       <c r="B8" t="n">
-        <v>0.1668548507162778</v>
+        <v>-0.7471526372682664</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.1425711349360504</v>
+        <v>-0.8581633615996517</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.1186925649371877</v>
+        <v>-0.8681092109053035</v>
       </c>
       <c r="E8" t="n">
-        <v>0.09130602458666411</v>
+        <v>-0.8425804111809766</v>
       </c>
       <c r="F8" t="n">
-        <v>0.2234888283802195</v>
+        <v>-0.8001141319985793</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>exp2_cdwa_v0_a0_b0_w3_C4_r4.bag</t>
+          <t>exp3_cdwa1_w3_C4_r4.bag</t>
         </is>
       </c>
     </row>
@@ -598,23 +530,23 @@
         <v>5</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.6279856195737675</v>
+        <v>-0.665281799702523</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.80286380291054</v>
+        <v>-0.8057258371340386</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.6539607819306659</v>
+        <v>-0.6562080555191648</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2988400192556984</v>
+        <v>0.2800614058751336</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.6616453801437451</v>
+        <v>-0.6732711784899386</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>exp2_cdwa_v0_a0_b0_w3_C8_r0.bag</t>
+          <t>exp3_cdwa1_w3_C8_r0.bag</t>
         </is>
       </c>
     </row>
@@ -623,23 +555,23 @@
         <v>6</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.7547240916737824</v>
+        <v>-0.4848350264733896</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.7958116041519713</v>
+        <v>-0.6228208116816955</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.796917167026302</v>
+        <v>-0.7314117991825992</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.7002203203143668</v>
+        <v>-0.6986377160198806</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.7968075090525738</v>
+        <v>-0.5118210612256765</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>exp2_cdwa_v0_a0_b0_w3_C8_r1.bag</t>
+          <t>exp3_cdwa1_w3_C8_r1.bag</t>
         </is>
       </c>
     </row>
@@ -648,23 +580,23 @@
         <v>7</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.291893812256702</v>
+        <v>-0.4705917243547721</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.433382611561864</v>
+        <v>-0.6292998645976879</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.587134981825548</v>
+        <v>-0.6853596076287582</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.7689576396192814</v>
+        <v>-0.6199312715133094</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.339893654028956</v>
+        <v>-0.5279014313826627</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>exp2_cdwa_v0_a0_b0_w3_C8_r2.bag</t>
+          <t>exp3_cdwa1_w3_C8_r2.bag</t>
         </is>
       </c>
     </row>
@@ -673,23 +605,23 @@
         <v>8</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.7843033562719958</v>
+        <v>-0.7985404213354906</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.8203670585173823</v>
+        <v>-0.8352846075245539</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.7576565923660344</v>
+        <v>-0.7623068358105568</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.4550358067398749</v>
+        <v>-0.4018847798969204</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.7741485757675072</v>
+        <v>-0.794006674163796</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>exp2_cdwa_v0_a0_b0_w3_C8_r3.bag</t>
+          <t>exp3_cdwa1_w3_C8_r3.bag</t>
         </is>
       </c>
     </row>
@@ -698,23 +630,23 @@
         <v>9</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.948453209932392</v>
+        <v>-0.931026362235881</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.9418290959475941</v>
+        <v>-0.9507707963141869</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.8871990209231945</v>
+        <v>-0.8761150428779862</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.8081423474469517</v>
+        <v>-0.7997713793771809</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.9481509060192193</v>
+        <v>-0.9296885435793761</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>exp2_cdwa_v0_a0_b0_w3_C8_r4.bag</t>
+          <t>exp3_cdwa1_w3_C8_r4.bag</t>
         </is>
       </c>
     </row>
@@ -723,23 +655,23 @@
         <v>10</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.2340051894328218</v>
+        <v>-0.8035936605379675</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.4004692230952146</v>
+        <v>-0.6150892744134782</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.6332176444322363</v>
+        <v>-0.3467839242597464</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.8212348923672338</v>
+        <v>-0.1727501786359029</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.2486982754782361</v>
+        <v>-0.7587239428053292</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>exp2_cdwa_v0_a0_b0_w4_C4_r0.bag</t>
+          <t>exp3_cdwa1_w4_C4_r0.bag</t>
         </is>
       </c>
     </row>
@@ -748,23 +680,23 @@
         <v>11</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.3488670244593737</v>
+        <v>-0.2982551266058114</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.4452373825587297</v>
+        <v>-0.6265152534246134</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.625293760985576</v>
+        <v>-0.8234341956624245</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.74528205008088</v>
+        <v>-0.8952555486569849</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.4271224923801913</v>
+        <v>-0.2067538804195689</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>exp2_cdwa_v0_a0_b0_w4_C4_r1.bag</t>
+          <t>exp3_cdwa1_w4_C4_r1.bag</t>
         </is>
       </c>
     </row>
@@ -773,23 +705,23 @@
         <v>12</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.3407817333716594</v>
+        <v>-0.367638173200275</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.5886640053059445</v>
+        <v>-0.6113148475098945</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.6778499810235357</v>
+        <v>-0.6532333312306599</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.8651314859888805</v>
+        <v>-0.8607426421260935</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.3875787631608886</v>
+        <v>-0.4051541979841365</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>exp2_cdwa_v0_a0_b0_w4_C4_r2.bag</t>
+          <t>exp3_cdwa1_w4_C4_r2.bag</t>
         </is>
       </c>
     </row>
@@ -798,23 +730,23 @@
         <v>13</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.3291140895547239</v>
+        <v>0.2542959944535256</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.4029060859487258</v>
+        <v>0.3900681680566253</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.4984911638344412</v>
+        <v>-0.597894267613539</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.5747727309049411</v>
+        <v>-0.6728806846632656</v>
       </c>
       <c r="F17" t="n">
-        <v>0.4527878505785109</v>
+        <v>0.3679301498708003</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>exp2_cdwa_v0_a0_b0_w4_C4_r3.bag</t>
+          <t>exp3_cdwa1_w4_C4_r3.bag</t>
         </is>
       </c>
     </row>
@@ -823,23 +755,23 @@
         <v>14</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.6609618221045014</v>
+        <v>-0.6560561650594285</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.7098380286710902</v>
+        <v>-0.7241762258201195</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.7812226988851534</v>
+        <v>-0.7952114182753782</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.7683336512132882</v>
+        <v>-0.7921233265666138</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.6864075561307843</v>
+        <v>-0.6872127552874909</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>exp2_cdwa_v0_a0_b0_w4_C4_r4.bag</t>
+          <t>exp3_cdwa1_w4_C4_r4.bag</t>
         </is>
       </c>
     </row>
@@ -848,23 +780,23 @@
         <v>15</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.8104880672055799</v>
+        <v>-0.808200448917245</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.8944561816860691</v>
+        <v>-0.8991036442135437</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.8040814306434768</v>
+        <v>-0.8083167580656001</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.6122583579342619</v>
+        <v>-0.6287347071893497</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.8148598381322973</v>
+        <v>-0.8090974155071581</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>exp2_cdwa_v0_a0_b0_w4_C8_r0.bag</t>
+          <t>exp3_cdwa1_w4_C8_r0.bag</t>
         </is>
       </c>
     </row>
@@ -873,23 +805,23 @@
         <v>16</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.5065604845582604</v>
+        <v>-0.4330522074341633</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.6418678805978926</v>
+        <v>-0.5805098481779875</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.7205522880198729</v>
+        <v>-0.693965518036944</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.7396559130218574</v>
+        <v>-0.7074790217815058</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.4937699035119365</v>
+        <v>-0.4304771318350327</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>exp2_cdwa_v0_a0_b0_w4_C8_r1.bag</t>
+          <t>exp3_cdwa1_w4_C8_r1.bag</t>
         </is>
       </c>
     </row>
@@ -898,23 +830,23 @@
         <v>17</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.5913863797429414</v>
+        <v>-0.5674063411074832</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.7075469057164808</v>
+        <v>-0.7027551758585761</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.716100424871859</v>
+        <v>-0.7049881677435962</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.8169377821031198</v>
+        <v>-0.8162605525629311</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.5326959145402742</v>
+        <v>-0.5096757580489818</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>exp2_cdwa_v0_a0_b0_w4_C8_r2.bag</t>
+          <t>exp3_cdwa1_w4_C8_r2.bag</t>
         </is>
       </c>
     </row>
@@ -923,23 +855,23 @@
         <v>18</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.4893943810128832</v>
+        <v>-0.5088989650291121</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.6964264815820685</v>
+        <v>-0.7115117971173978</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.790276877809761</v>
+        <v>-0.7830673043554186</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.8561726752182324</v>
+        <v>-0.8637539757257153</v>
       </c>
       <c r="F22" t="n">
-        <v>-0.4981017169453154</v>
+        <v>-0.5032496601174382</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>exp2_cdwa_v0_a0_b0_w4_C8_r3.bag</t>
+          <t>exp3_cdwa1_w4_C8_r3.bag</t>
         </is>
       </c>
     </row>
@@ -948,23 +880,23 @@
         <v>19</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.6212946417003965</v>
+        <v>-0.6849711479818195</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.7406798974841481</v>
+        <v>-0.7526202160098286</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.6669559896573565</v>
+        <v>-0.5749744164490402</v>
       </c>
       <c r="E23" t="n">
-        <v>-0.6639322781830338</v>
+        <v>-0.7243958293798345</v>
       </c>
       <c r="F23" t="n">
-        <v>-0.5462209531753822</v>
+        <v>-0.6473955811266633</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>exp2_cdwa_v0_a0_b0_w4_C8_r4.bag</t>
+          <t>exp3_cdwa1_w4_C8_r4.bag</t>
         </is>
       </c>
     </row>

</xml_diff>